<commit_message>
adding files week 6
</commit_message>
<xml_diff>
--- a/CSE 300/StudentTrackingAssignments.xlsx
+++ b/CSE 300/StudentTrackingAssignments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alejo\Desktop\FAMILIA\Alejo\TECH\developments\PERSONAL DEVELOPMENTS\Machine-learning-projects\CSE 300\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538FEF5B-918F-406B-B51E-756EF4621008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B70CDF-E18E-4B43-83BE-BC2C9D6598B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" tabRatio="875" activeTab="3" xr2:uid="{07D90E1F-7C1C-A043-A0EA-0FD351459508}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" tabRatio="875" activeTab="10" xr2:uid="{07D90E1F-7C1C-A043-A0EA-0FD351459508}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="A7_Status" sheetId="25" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">A0_Plan!$A$1:$R$68</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">A0_Plan!$A$1:$R$82</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">A1_Status!$C$1:$H$51</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">A2_Status!$B$1:$H$51</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="6">A3_Status!$A$1:$H$51</definedName>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="361">
   <si>
     <t>Issues</t>
   </si>
@@ -1299,6 +1299,42 @@
   </si>
   <si>
     <t>get an interview</t>
+  </si>
+  <si>
+    <t>https://github.com/AlejoAlegreBustos/Machine-learning-projects</t>
+  </si>
+  <si>
+    <t>https://github.com/AlejoAlegreBustos/Machine-learning-projects/blob/main/CSE%20300/job%20application%203.png</t>
+  </si>
+  <si>
+    <t>https://github.com/AlejoAlegreBustos/Machine-learning-projects/blob/main/CSE%20300/251013_Alejo%20Alegre%20Bustos_002.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/AlejoAlegreBustos/Machine-learning-projects/blob/main/CSE%20300/vmock%20interviews.png</t>
+  </si>
+  <si>
+    <t>https://github.com/AlejoAlegreBustos/Machine-learning-projects/blob/main/CSE%20300/informational%20interview%203.png</t>
+  </si>
+  <si>
+    <t>The first four chapters of The 2-Hour Job Search are all about working smarter when job hunting. Instead of sending your résumé everywhere and hoping for luck, Steve Dalton shows a faster way using the LAMP method — List, Alumni, Motivation, and Posting. Basically, you make a list of companies you’d like to work for, see where you’ve got some kind of connection, check which ones actually interest you, and note if they’ve got open roles. Then you rank them, so you know where to start reaching out. It’s a simple system that takes a couple of hours to set up but makes the whole job search way more focused and less stressful.</t>
+  </si>
+  <si>
+    <t>great wat to practice coding, also, it is a excellente way to lear before hand in which branch of data science I would like to work</t>
+  </si>
+  <si>
+    <t>great way to practice and lose the fear or insecurity that you feel before the interview</t>
+  </si>
+  <si>
+    <t>this time I learn what that informational interviews are great way to know what life style you can have in certain companies</t>
+  </si>
+  <si>
+    <t>In class</t>
+  </si>
+  <si>
+    <t>Placeholder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I interviewed Murphy USA, a gas copany, in this case we had the visit of the data and software engineering team, I asked a couple of questions about how is the company implementing math models or ML models in the context of AI </t>
   </si>
 </sst>
 </file>
@@ -3453,7 +3489,7 @@
       </c>
       <c r="H6" s="37">
         <f>Backlog!H5</f>
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.5">
@@ -3482,7 +3518,7 @@
       </c>
       <c r="C8" s="15">
         <f>Backlog!G3</f>
-        <v>0.84615384615384615</v>
+        <v>0.87179487179487181</v>
       </c>
       <c r="D8">
         <f>SUM(A0_Plan!H15:H69)</f>
@@ -3716,11 +3752,11 @@
       </c>
       <c r="D18">
         <f>A5_Status!G18</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E18" s="39">
         <f>A5_Status!G19</f>
-        <v>0</v>
+        <v>2.3333333333333335</v>
       </c>
       <c r="G18" s="33" t="s">
         <v>187</v>
@@ -3756,11 +3792,11 @@
       </c>
       <c r="D19">
         <f>A6_Status!G18</f>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="E19" s="39">
         <f>A6_Status!G19</f>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="G19" s="33" t="s">
         <v>188</v>
@@ -3796,11 +3832,11 @@
       </c>
       <c r="D20">
         <f>A7_Status!G18</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="39">
         <f>A7_Status!G19</f>
-        <v>0</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="G20" s="33" t="s">
         <v>189</v>
@@ -3844,8 +3880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8515058B-4DE2-4DB6-8AD2-37BD43F2C8C4}">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="C6" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="110" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -3958,8 +3994,12 @@
         <f>IF(ISBLANK(A0_Plan!F53),"",A0_Plan!F53)</f>
         <v/>
       </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="F11" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G11" s="7">
+        <v>0.5</v>
+      </c>
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.5">
@@ -3974,9 +4014,15 @@
         <f>IF(ISBLANK(A0_Plan!F54),"",A0_Plan!F54)</f>
         <v/>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="F12" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G12" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>359</v>
+      </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.5">
       <c r="C13">
@@ -3984,14 +4030,18 @@
       </c>
       <c r="D13" t="str">
         <f>IF(ISBLANK(A0_Plan!E55),"",A0_Plan!E55)</f>
-        <v>23_J2_Network Contact List</v>
+        <v>6_S1_Scheduled Silver Meeting with Career Services</v>
       </c>
       <c r="E13" t="str">
         <f>IF(ISBLANK(A0_Plan!F55),"",A0_Plan!F55)</f>
         <v/>
       </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
+      <c r="F13" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G13" s="7">
+        <v>0.5</v>
+      </c>
       <c r="H13" s="7"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.5">
@@ -4015,15 +4065,21 @@
       </c>
       <c r="D15" t="str">
         <f>IF(ISBLANK(A0_Plan!E57),"",A0_Plan!E57)</f>
-        <v>22_J1_Networking List</v>
+        <v>24_J3_Company Dossiers</v>
       </c>
       <c r="E15" t="str">
         <f>IF(ISBLANK(A0_Plan!F57),"",A0_Plan!F57)</f>
         <v/>
       </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
+      <c r="F15" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G15" s="7">
+        <v>1</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.5">
       <c r="C16">
@@ -4037,9 +4093,15 @@
         <f>IF(ISBLANK(A0_Plan!F58),"",A0_Plan!F58)</f>
         <v/>
       </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
+      <c r="F16" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G16" s="7">
+        <v>1</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C17">
@@ -4053,9 +4115,15 @@
         <f>IF(ISBLANK(A0_Plan!F59),"",A0_Plan!F59)</f>
         <v/>
       </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
+      <c r="F17" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G17" s="7">
+        <v>1</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.5">
       <c r="D18" s="27" t="s">
@@ -4068,7 +4136,7 @@
       <c r="F18" s="28"/>
       <c r="G18" s="28">
         <f>SUM(G11:G17)</f>
-        <v>0</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.5">
@@ -4082,7 +4150,7 @@
       <c r="F19" s="28"/>
       <c r="G19" s="28">
         <f>G18/6</f>
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="20" spans="3:8" ht="21" x14ac:dyDescent="0.65">
@@ -4117,7 +4185,7 @@
       </c>
       <c r="D23" t="str">
         <f>IF(ISBLANK(A0_Plan!E62),"",A0_Plan!E62)</f>
-        <v>24_J3_Company Dossiers</v>
+        <v>22_J1_Networking List</v>
       </c>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.5">
@@ -4162,7 +4230,7 @@
       </c>
       <c r="D28" t="str">
         <f>IF(ISBLANK(A0_Plan!E67),"",A0_Plan!E67)</f>
-        <v>6_S1_Scheduled Silver Meeting with Career Services</v>
+        <v>23_J2_Network Contact List</v>
       </c>
     </row>
     <row r="29" spans="3:8" ht="21.4" thickBot="1" x14ac:dyDescent="0.7">
@@ -4383,17 +4451,17 @@
     <protectedRange sqref="F11:H13" name="Week 1 Day Status"/>
   </protectedRanges>
   <mergeCells count="11">
+    <mergeCell ref="E42:H42"/>
+    <mergeCell ref="C47:H47"/>
+    <mergeCell ref="D49:H49"/>
+    <mergeCell ref="D50:H50"/>
+    <mergeCell ref="D51:H51"/>
     <mergeCell ref="E39:H39"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="C6:H6"/>
     <mergeCell ref="D30:H33"/>
     <mergeCell ref="C36:H36"/>
     <mergeCell ref="E38:H38"/>
-    <mergeCell ref="E42:H42"/>
-    <mergeCell ref="C47:H47"/>
-    <mergeCell ref="D49:H49"/>
-    <mergeCell ref="D50:H50"/>
-    <mergeCell ref="D51:H51"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F11:F13 F15:F17" xr:uid="{A2A76FCC-8F65-48BC-A8F4-A01273D51EE7}">
@@ -4412,8 +4480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9622B604-494A-4C6C-A562-4F39848323A4}">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="C6" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="110" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -4526,9 +4594,15 @@
         <f>IF(ISBLANK(A0_Plan!F61),"",A0_Plan!F61)</f>
         <v/>
       </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="F11" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G11" s="7">
+        <v>1</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.5">
       <c r="C12">
@@ -4536,7 +4610,7 @@
       </c>
       <c r="D12" t="str">
         <f>IF(ISBLANK(A0_Plan!E62),"",A0_Plan!E62)</f>
-        <v>24_J3_Company Dossiers</v>
+        <v>22_J1_Networking List</v>
       </c>
       <c r="E12" t="str">
         <f>IF(ISBLANK(A0_Plan!F62),"",A0_Plan!F62)</f>
@@ -4615,7 +4689,7 @@
       </c>
       <c r="D17" t="str">
         <f>IF(ISBLANK(A0_Plan!E67),"",A0_Plan!E67)</f>
-        <v>6_S1_Scheduled Silver Meeting with Career Services</v>
+        <v>23_J2_Network Contact List</v>
       </c>
       <c r="E17" t="str">
         <f>IF(ISBLANK(A0_Plan!F67),"",A0_Plan!F67)</f>
@@ -4636,7 +4710,7 @@
       <c r="F18" s="28"/>
       <c r="G18" s="28">
         <f>SUM(G11:G17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.5">
@@ -4650,7 +4724,7 @@
       <c r="F19" s="28"/>
       <c r="G19" s="28">
         <f>G18/6</f>
-        <v>0</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="20" spans="3:8" ht="21" x14ac:dyDescent="0.65">
@@ -4934,17 +5008,17 @@
     <protectedRange sqref="F11:H13" name="Week 1 Day Status"/>
   </protectedRanges>
   <mergeCells count="11">
+    <mergeCell ref="E42:H42"/>
+    <mergeCell ref="C47:H47"/>
+    <mergeCell ref="D49:H49"/>
+    <mergeCell ref="D50:H50"/>
+    <mergeCell ref="D51:H51"/>
     <mergeCell ref="E39:H39"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="C6:H6"/>
     <mergeCell ref="D30:H33"/>
     <mergeCell ref="C36:H36"/>
     <mergeCell ref="E38:H38"/>
-    <mergeCell ref="E42:H42"/>
-    <mergeCell ref="C47:H47"/>
-    <mergeCell ref="D49:H49"/>
-    <mergeCell ref="D50:H50"/>
-    <mergeCell ref="D51:H51"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F11:F13 F15:F17" xr:uid="{D1B2BB17-8A06-4144-A681-8A997469D79E}">
@@ -5778,7 +5852,7 @@
       </c>
       <c r="G3" s="15">
         <f>AVERAGEA(G4:G47)</f>
-        <v>0.84615384615384615</v>
+        <v>0.87179487179487181</v>
       </c>
       <c r="I3" s="15"/>
       <c r="K3" s="15"/>
@@ -5829,7 +5903,7 @@
       <c r="F5" s="13"/>
       <c r="H5" s="37">
         <f>AVERAGEA(G6:G10)</f>
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.5">
@@ -5950,9 +6024,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G9" s="6" t="str">
+      <c r="G9" s="6">
         <f>IF(VLOOKUP(D9,A0_Plan!$E$13:$K$67,5,1)="Done", 1,"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="H9" s="6"/>
       <c r="J9" s="6"/>
@@ -7253,8 +7327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E5406B-F50C-854D-9060-592EBAE21E85}">
   <dimension ref="B1:Q68"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A46" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="N64" sqref="N64"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A49" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -8334,17 +8408,17 @@
         <f>IF(F45&gt;0, 1,0)</f>
         <v>0</v>
       </c>
-      <c r="I45">
+      <c r="I45" t="str">
         <f>A5_Status!F11</f>
-        <v>0</v>
+        <v>Working</v>
       </c>
       <c r="J45">
         <f>A5_Status!G11</f>
-        <v>0</v>
-      </c>
-      <c r="K45">
+        <v>10</v>
+      </c>
+      <c r="K45" t="str">
         <f>A5_Status!H11</f>
-        <v>0</v>
+        <v>https://github.com/AlejoAlegreBustos/Machine-learning-projects</v>
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.5">
@@ -8366,17 +8440,17 @@
         <f>IF(F46&gt;0, 1,0)</f>
         <v>0</v>
       </c>
-      <c r="I46">
+      <c r="I46" t="str">
         <f>A5_Status!F12</f>
-        <v>0</v>
+        <v>Done</v>
       </c>
       <c r="J46">
         <f>A5_Status!G12</f>
-        <v>0</v>
-      </c>
-      <c r="K46">
+        <v>1</v>
+      </c>
+      <c r="K46" t="str">
         <f>A5_Status!H12</f>
-        <v>0</v>
+        <v>https://github.com/AlejoAlegreBustos/Machine-learning-projects/blob/main/CSE%20300/vmock%20interviews.png</v>
       </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.5">
@@ -8398,17 +8472,17 @@
         <f>IF(F47&gt;0, 1,0)</f>
         <v>0</v>
       </c>
-      <c r="I47">
+      <c r="I47" t="str">
         <f>A5_Status!F13</f>
-        <v>0</v>
+        <v>Done</v>
       </c>
       <c r="J47">
         <f>A5_Status!G13</f>
-        <v>0</v>
-      </c>
-      <c r="K47">
+        <v>1.5</v>
+      </c>
+      <c r="K47" t="str">
         <f>A5_Status!H13</f>
-        <v>0</v>
+        <v>The first four chapters of The 2-Hour Job Search are all about working smarter when job hunting. Instead of sending your résumé everywhere and hoping for luck, Steve Dalton shows a faster way using the LAMP method — List, Alumni, Motivation, and Posting. Basically, you make a list of companies you’d like to work for, see where you’ve got some kind of connection, check which ones actually interest you, and note if they’ve got open roles. Then you rank them, so you know where to start reaching out. It’s a simple system that takes a couple of hours to set up but makes the whole job search way more focused and less stressful.</v>
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.5">
@@ -8430,17 +8504,17 @@
         <f>IF(F49&gt;0, 1,0)</f>
         <v>0</v>
       </c>
-      <c r="I49">
+      <c r="I49" t="str">
         <f>A5_Status!F15</f>
-        <v>0</v>
+        <v>Done</v>
       </c>
       <c r="J49">
         <f>A5_Status!G15</f>
-        <v>0</v>
-      </c>
-      <c r="K49">
+        <v>0.5</v>
+      </c>
+      <c r="K49" t="str">
         <f>A5_Status!H15</f>
-        <v>0</v>
+        <v>https://github.com/AlejoAlegreBustos/Machine-learning-projects/blob/main/CSE%20300/informational%20interview%203.png</v>
       </c>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.5">
@@ -8462,17 +8536,17 @@
         <f>IF(F50&gt;0, 1,0)</f>
         <v>0</v>
       </c>
-      <c r="I50">
+      <c r="I50" t="str">
         <f>A5_Status!F16</f>
-        <v>0</v>
+        <v>Done</v>
       </c>
       <c r="J50">
         <f>A5_Status!G16</f>
-        <v>0</v>
-      </c>
-      <c r="K50">
+        <v>0.5</v>
+      </c>
+      <c r="K50" t="str">
         <f>A5_Status!H16</f>
-        <v>0</v>
+        <v>https://github.com/AlejoAlegreBustos/Machine-learning-projects/blob/main/CSE%20300/251013_Alejo%20Alegre%20Bustos_002.jpg</v>
       </c>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.5">
@@ -8494,17 +8568,17 @@
         <f>IF(F51&gt;0, 1,0)</f>
         <v>0</v>
       </c>
-      <c r="I51">
+      <c r="I51" t="str">
         <f>A5_Status!F17</f>
-        <v>0</v>
+        <v>Done</v>
       </c>
       <c r="J51">
         <f>A5_Status!G17</f>
-        <v>0</v>
-      </c>
-      <c r="K51">
+        <v>0.5</v>
+      </c>
+      <c r="K51" t="str">
         <f>A5_Status!H17</f>
-        <v>0</v>
+        <v>https://github.com/AlejoAlegreBustos/Machine-learning-projects/blob/main/CSE%20300/job%20application%203.png</v>
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.5">
@@ -8535,13 +8609,13 @@
         <f>IF(F53&gt;0, 1,0)</f>
         <v>0</v>
       </c>
-      <c r="I53">
+      <c r="I53" t="str">
         <f>A6_Status!F11</f>
-        <v>0</v>
+        <v>Done</v>
       </c>
       <c r="J53">
         <f>A6_Status!G11</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K53">
         <f>A6_Status!H11</f>
@@ -8567,17 +8641,17 @@
         <f>IF(F54&gt;0, 1,0)</f>
         <v>0</v>
       </c>
-      <c r="I54">
+      <c r="I54" t="str">
         <f>A6_Status!F12</f>
-        <v>0</v>
+        <v>Done</v>
       </c>
       <c r="J54">
         <f>A6_Status!G12</f>
-        <v>0</v>
-      </c>
-      <c r="K54">
+        <v>0.5</v>
+      </c>
+      <c r="K54" t="str">
         <f>A6_Status!H12</f>
-        <v>0</v>
+        <v>Placeholder</v>
       </c>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.5">
@@ -8588,7 +8662,7 @@
         <v>3</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
       <c r="F55" s="7"/>
       <c r="G55" t="str">
@@ -8599,13 +8673,13 @@
         <f>IF(F55&gt;0, 1,0)</f>
         <v>0</v>
       </c>
-      <c r="I55">
+      <c r="I55" t="str">
         <f>A6_Status!F13</f>
-        <v>0</v>
+        <v>Done</v>
       </c>
       <c r="J55">
         <f>A6_Status!G13</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K55">
         <f>A6_Status!H13</f>
@@ -8620,7 +8694,7 @@
         <v>1</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
       <c r="F57" s="7"/>
       <c r="G57" t="str">
@@ -8631,17 +8705,17 @@
         <f>IF(F57&gt;0, 1,0)</f>
         <v>0</v>
       </c>
-      <c r="I57">
+      <c r="I57" t="str">
         <f>A6_Status!F15</f>
-        <v>0</v>
+        <v>Done</v>
       </c>
       <c r="J57">
         <f>A6_Status!G15</f>
-        <v>0</v>
-      </c>
-      <c r="K57">
+        <v>1</v>
+      </c>
+      <c r="K57" t="str">
         <f>A6_Status!H15</f>
-        <v>0</v>
+        <v>In class</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.5">
@@ -8663,17 +8737,17 @@
         <f>IF(F58&gt;0, 1,0)</f>
         <v>0</v>
       </c>
-      <c r="I58">
+      <c r="I58" t="str">
         <f>A6_Status!F16</f>
-        <v>0</v>
+        <v>Done</v>
       </c>
       <c r="J58">
         <f>A6_Status!G16</f>
-        <v>0</v>
-      </c>
-      <c r="K58">
+        <v>1</v>
+      </c>
+      <c r="K58" t="str">
         <f>A6_Status!H16</f>
-        <v>0</v>
+        <v>In class</v>
       </c>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.5">
@@ -8695,17 +8769,17 @@
         <f>IF(F59&gt;0, 1,0)</f>
         <v>0</v>
       </c>
-      <c r="I59">
+      <c r="I59" t="str">
         <f>A6_Status!F17</f>
-        <v>0</v>
+        <v>Done</v>
       </c>
       <c r="J59">
         <f>A6_Status!G17</f>
-        <v>0</v>
-      </c>
-      <c r="K59">
+        <v>1</v>
+      </c>
+      <c r="K59" t="str">
         <f>A6_Status!H17</f>
-        <v>0</v>
+        <v>In class</v>
       </c>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.5">
@@ -8736,17 +8810,17 @@
         <f>IF(F61&gt;0, 1,0)</f>
         <v>0</v>
       </c>
-      <c r="I61">
+      <c r="I61" t="str">
         <f>A7_Status!F11</f>
-        <v>0</v>
+        <v>Done</v>
       </c>
       <c r="J61">
         <f>A7_Status!G11</f>
-        <v>0</v>
-      </c>
-      <c r="K61">
+        <v>1</v>
+      </c>
+      <c r="K61" t="str">
         <f>A7_Status!H11</f>
-        <v>0</v>
+        <v xml:space="preserve">I interviewed Murphy USA, a gas copany, in this case we had the visit of the data and software engineering team, I asked a couple of questions about how is the company implementing math models or ML models in the context of AI </v>
       </c>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.5">
@@ -8757,7 +8831,7 @@
         <v>2</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>299</v>
+        <v>279</v>
       </c>
       <c r="F62" s="7"/>
       <c r="G62" t="str">
@@ -8885,7 +8959,7 @@
         <v>3</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>276</v>
+        <v>294</v>
       </c>
       <c r="F67" s="7"/>
       <c r="G67" t="str">
@@ -9540,11 +9614,6 @@
     <protectedRange sqref="F11:H13" name="Week 1 Day Status"/>
   </protectedRanges>
   <mergeCells count="14">
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="C36:H36"/>
-    <mergeCell ref="D49:H49"/>
-    <mergeCell ref="D50:H50"/>
     <mergeCell ref="D51:H51"/>
     <mergeCell ref="D30:H33"/>
     <mergeCell ref="C47:H47"/>
@@ -9554,6 +9623,11 @@
     <mergeCell ref="E40:H40"/>
     <mergeCell ref="E44:H44"/>
     <mergeCell ref="E43:H43"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C36:H36"/>
+    <mergeCell ref="D49:H49"/>
+    <mergeCell ref="D50:H50"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F11:F13 F15:F17" xr:uid="{F8BA5BF8-27F7-0145-ACE8-38CF1DEED6A9}">
@@ -10162,6 +10236,12 @@
     <protectedRange sqref="F11:H13" name="Week 1 Day Status"/>
   </protectedRanges>
   <mergeCells count="13">
+    <mergeCell ref="C47:H47"/>
+    <mergeCell ref="D49:H49"/>
+    <mergeCell ref="D50:H50"/>
+    <mergeCell ref="D51:H51"/>
+    <mergeCell ref="E43:H43"/>
+    <mergeCell ref="E44:H44"/>
     <mergeCell ref="E40:H40"/>
     <mergeCell ref="E39:H39"/>
     <mergeCell ref="C4:H4"/>
@@ -10169,12 +10249,6 @@
     <mergeCell ref="D30:H33"/>
     <mergeCell ref="C36:H36"/>
     <mergeCell ref="E38:H38"/>
-    <mergeCell ref="C47:H47"/>
-    <mergeCell ref="D49:H49"/>
-    <mergeCell ref="D50:H50"/>
-    <mergeCell ref="D51:H51"/>
-    <mergeCell ref="E43:H43"/>
-    <mergeCell ref="E44:H44"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F11:F13 F15:F17" xr:uid="{0C4CAE71-73BA-45BA-B81A-F9DB73364F6C}">
@@ -10778,18 +10852,18 @@
     <protectedRange sqref="F11:H11 F13:H13 F12:G12" name="Week 1 Day Status"/>
   </protectedRanges>
   <mergeCells count="12">
+    <mergeCell ref="E42:H42"/>
+    <mergeCell ref="C47:H47"/>
+    <mergeCell ref="D49:H49"/>
+    <mergeCell ref="D50:H50"/>
+    <mergeCell ref="D51:H51"/>
+    <mergeCell ref="E44:H44"/>
     <mergeCell ref="E39:H39"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="C6:H6"/>
     <mergeCell ref="D30:H33"/>
     <mergeCell ref="C36:H36"/>
     <mergeCell ref="E38:H38"/>
-    <mergeCell ref="E42:H42"/>
-    <mergeCell ref="C47:H47"/>
-    <mergeCell ref="D49:H49"/>
-    <mergeCell ref="D50:H50"/>
-    <mergeCell ref="D51:H51"/>
-    <mergeCell ref="E44:H44"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F11:F13 F15:F17" xr:uid="{B26C00AE-C8F1-4A9E-BD78-2336D2567EF8}">
@@ -10808,8 +10882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19E3BF9B-6B9F-4347-A3C9-CC5DD92EABEF}">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView topLeftCell="A44" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="110" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49:H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -11400,17 +11474,17 @@
     <protectedRange sqref="F11:H13" name="Week 1 Day Status"/>
   </protectedRanges>
   <mergeCells count="11">
+    <mergeCell ref="E42:H42"/>
+    <mergeCell ref="C47:H47"/>
+    <mergeCell ref="D49:H49"/>
+    <mergeCell ref="D50:H50"/>
+    <mergeCell ref="D51:H51"/>
     <mergeCell ref="E39:H39"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="C6:H6"/>
     <mergeCell ref="D30:H33"/>
     <mergeCell ref="C36:H36"/>
     <mergeCell ref="E38:H38"/>
-    <mergeCell ref="E42:H42"/>
-    <mergeCell ref="C47:H47"/>
-    <mergeCell ref="D49:H49"/>
-    <mergeCell ref="D50:H50"/>
-    <mergeCell ref="D51:H51"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F11:F13 F15:F17" xr:uid="{A4DED5BE-B352-4550-8DBB-9F1D1D8AB303}">
@@ -11430,7 +11504,7 @@
   <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D11" sqref="D11:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -11543,9 +11617,15 @@
         <f>IF(ISBLANK(A0_Plan!F45),"",A0_Plan!F45)</f>
         <v/>
       </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="F11" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="G11" s="7">
+        <v>10</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.5">
       <c r="C12">
@@ -11559,9 +11639,15 @@
         <f>IF(ISBLANK(A0_Plan!F46),"",A0_Plan!F46)</f>
         <v/>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="F12" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G12" s="7">
+        <v>1</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.5">
       <c r="C13">
@@ -11575,9 +11661,15 @@
         <f>IF(ISBLANK(A0_Plan!F47),"",A0_Plan!F47)</f>
         <v/>
       </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="F13" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G13" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.5">
       <c r="C14" t="s">
@@ -11606,9 +11698,15 @@
         <f>IF(ISBLANK(A0_Plan!F49),"",A0_Plan!F49)</f>
         <v/>
       </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
+      <c r="F15" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G15" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.5">
       <c r="C16">
@@ -11622,9 +11720,15 @@
         <f>IF(ISBLANK(A0_Plan!F50),"",A0_Plan!F50)</f>
         <v/>
       </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
+      <c r="F16" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G16" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>351</v>
+      </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.5">
       <c r="C17">
@@ -11638,9 +11742,15 @@
         <f>IF(ISBLANK(A0_Plan!F51),"",A0_Plan!F51)</f>
         <v/>
       </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
+      <c r="F17" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G17" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>350</v>
+      </c>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.5">
       <c r="D18" s="27" t="s">
@@ -11653,7 +11763,7 @@
       <c r="F18" s="28"/>
       <c r="G18" s="28">
         <f>SUM(G11:G17)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.5">
@@ -11667,7 +11777,7 @@
       <c r="F19" s="28"/>
       <c r="G19" s="28">
         <f>G18/6</f>
-        <v>0</v>
+        <v>2.3333333333333335</v>
       </c>
     </row>
     <row r="20" spans="3:8" ht="21" x14ac:dyDescent="0.65">
@@ -11711,7 +11821,7 @@
       </c>
       <c r="D24" t="str">
         <f>IF(ISBLANK(A0_Plan!E55),"",A0_Plan!E55)</f>
-        <v>23_J2_Network Contact List</v>
+        <v>6_S1_Scheduled Silver Meeting with Career Services</v>
       </c>
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.5">
@@ -11729,7 +11839,7 @@
       </c>
       <c r="D26" t="str">
         <f>IF(ISBLANK(A0_Plan!E57),"",A0_Plan!E57)</f>
-        <v>22_J1_Networking List</v>
+        <v>24_J3_Company Dossiers</v>
       </c>
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.5">
@@ -11756,7 +11866,9 @@
       </c>
     </row>
     <row r="30" spans="3:8" x14ac:dyDescent="0.5">
-      <c r="D30" s="69"/>
+      <c r="D30" s="69" t="s">
+        <v>307</v>
+      </c>
       <c r="E30" s="70"/>
       <c r="F30" s="70"/>
       <c r="G30" s="70"/>
@@ -11821,11 +11933,12 @@
       <c r="C38" t="s">
         <v>115</v>
       </c>
-      <c r="D38" t="str">
-        <f>IF(ISBLANK(A0_Plan!E13),"",A0_Plan!E13)</f>
-        <v>0_PP1_Planning Schedule</v>
-      </c>
-      <c r="E38" s="66"/>
+      <c r="D38" t="s">
+        <v>262</v>
+      </c>
+      <c r="E38" s="66" t="s">
+        <v>355</v>
+      </c>
       <c r="F38" s="67"/>
       <c r="G38" s="67"/>
       <c r="H38" s="68"/>
@@ -11834,11 +11947,12 @@
       <c r="C39" t="s">
         <v>116</v>
       </c>
-      <c r="D39" t="str">
-        <f>IF(ISBLANK(A0_Plan!E14),"",A0_Plan!E14)</f>
-        <v>17_P2_Resume</v>
-      </c>
-      <c r="E39" s="66"/>
+      <c r="D39" t="s">
+        <v>273</v>
+      </c>
+      <c r="E39" s="66" t="s">
+        <v>356</v>
+      </c>
       <c r="F39" s="67"/>
       <c r="G39" s="67"/>
       <c r="H39" s="68"/>
@@ -11847,11 +11961,12 @@
       <c r="C40" t="s">
         <v>117</v>
       </c>
-      <c r="D40" t="str">
-        <f>IF(ISBLANK(A0_Plan!E15),"",A0_Plan!E15)</f>
-        <v>31_D3_Design Your Life: Chap 1: Health, Work, Play, &amp; Love</v>
-      </c>
-      <c r="E40" s="24"/>
+      <c r="D40" t="s">
+        <v>288</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>354</v>
+      </c>
       <c r="F40" s="25"/>
       <c r="G40" s="25"/>
       <c r="H40" s="26"/>
@@ -11865,11 +11980,12 @@
       <c r="C42" t="s">
         <v>172</v>
       </c>
-      <c r="D42" t="str">
-        <f>IF(ISBLANK(A0_Plan!E17),"",A0_Plan!E17)</f>
-        <v>5_B5_Elevator Pitch: 5 Sentences</v>
-      </c>
-      <c r="E42" s="66"/>
+      <c r="D42" t="s">
+        <v>281</v>
+      </c>
+      <c r="E42" s="66" t="s">
+        <v>357</v>
+      </c>
       <c r="F42" s="67"/>
       <c r="G42" s="67"/>
       <c r="H42" s="68"/>
@@ -11878,9 +11994,8 @@
       <c r="C43" t="s">
         <v>173</v>
       </c>
-      <c r="D43" t="str">
-        <f>IF(ISBLANK(A0_Plan!E18),"",A0_Plan!E18)</f>
-        <v>32_D4_Design Your Life: Chap 2: Work/Life view/compass</v>
+      <c r="D43" t="s">
+        <v>268</v>
       </c>
       <c r="E43" s="21"/>
       <c r="F43" s="22"/>
@@ -11891,9 +12006,8 @@
       <c r="C44" t="s">
         <v>174</v>
       </c>
-      <c r="D44" t="str">
-        <f>IF(ISBLANK(A0_Plan!E19),"",A0_Plan!E19)</f>
-        <v>9_S4_Completed 100% Handshake Profile</v>
+      <c r="D44" t="s">
+        <v>297</v>
       </c>
       <c r="E44" s="21"/>
       <c r="F44" s="22"/>
@@ -11937,7 +12051,9 @@
       <c r="C49" t="s">
         <v>120</v>
       </c>
-      <c r="D49" s="66"/>
+      <c r="D49" s="66" t="s">
+        <v>314</v>
+      </c>
       <c r="E49" s="67"/>
       <c r="F49" s="67"/>
       <c r="G49" s="67"/>
@@ -11947,7 +12063,9 @@
       <c r="C50" t="s">
         <v>121</v>
       </c>
-      <c r="D50" s="66"/>
+      <c r="D50" s="66" t="s">
+        <v>315</v>
+      </c>
       <c r="E50" s="67"/>
       <c r="F50" s="67"/>
       <c r="G50" s="67"/>
@@ -11957,7 +12075,9 @@
       <c r="C51" t="s">
         <v>122</v>
       </c>
-      <c r="D51" s="66"/>
+      <c r="D51" s="66" t="s">
+        <v>348</v>
+      </c>
       <c r="E51" s="67"/>
       <c r="F51" s="67"/>
       <c r="G51" s="67"/>
@@ -11965,20 +12085,20 @@
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="F11:H13" name="Week 1 Day Status"/>
+    <protectedRange sqref="F11:H13 E40" name="Week 1 Day Status"/>
   </protectedRanges>
   <mergeCells count="11">
+    <mergeCell ref="E42:H42"/>
+    <mergeCell ref="C47:H47"/>
+    <mergeCell ref="D49:H49"/>
+    <mergeCell ref="D50:H50"/>
+    <mergeCell ref="D51:H51"/>
     <mergeCell ref="E39:H39"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="C6:H6"/>
     <mergeCell ref="D30:H33"/>
     <mergeCell ref="C36:H36"/>
     <mergeCell ref="E38:H38"/>
-    <mergeCell ref="E42:H42"/>
-    <mergeCell ref="C47:H47"/>
-    <mergeCell ref="D49:H49"/>
-    <mergeCell ref="D50:H50"/>
-    <mergeCell ref="D51:H51"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F11:F13 F15:F17" xr:uid="{F929D84E-5BAD-4824-868F-2008C632FB2D}">

</xml_diff>